<commit_message>
update variable efficiency input data
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/variable_efficiency_units.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/variable_efficiency_units.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5153D793-9290-42CA-A8B0-AFAABC20DBC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2815C4C-35F9-4FD2-8DD9-F85630BBD18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6F728511-B5BA-484C-BEF6-08D3CC388B55}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{6F728511-B5BA-484C-BEF6-08D3CC388B55}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable_Eff" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -475,7 +475,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -502,10 +502,10 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="C6">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -513,10 +513,10 @@
         <v>1</v>
       </c>
       <c r="B7">
-        <v>1.4285714285714286</v>
+        <v>0.7</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="C8">
         <v>1</v>

</xml_diff>

<commit_message>
fix variable efficiency bug in data prep
</commit_message>
<xml_diff>
--- a/spine_projects/01_input_data/01_input_raw/variable_efficiency_units.xlsx
+++ b/spine_projects/01_input_data/01_input_raw/variable_efficiency_units.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2815C4C-35F9-4FD2-8DD9-F85630BBD18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E25F1DF-6010-4BCD-8984-B89AB0F447D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{6F728511-B5BA-484C-BEF6-08D3CC388B55}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>unit__node__node</t>
   </si>
   <si>
-    <t>unit__to_node</t>
-  </si>
-  <si>
     <t>unit</t>
   </si>
   <si>
@@ -69,6 +66,9 @@
   </si>
   <si>
     <t>operating_points</t>
+  </si>
+  <si>
+    <t>unit__from_node</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -453,48 +453,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>